<commit_message>
Update Rizka - Lihat Status Pengajuan dan Ubah Foto Profil
</commit_message>
<xml_diff>
--- a/UbahFotoProfil.xlsx
+++ b/UbahFotoProfil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B02471-74EF-4EB8-AE27-6F8E16819941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D47C896-DACC-4185-92CD-70AA90BE6772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="0" windowWidth="17895" windowHeight="11070" xr2:uid="{B02B5606-CE9F-4185-A8EB-5B1A31EC9BA2}"/>
+    <workbookView xWindow="6105" yWindow="0" windowWidth="13440" windowHeight="11070" xr2:uid="{B02B5606-CE9F-4185-A8EB-5B1A31EC9BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>condition</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>passedRetake</t>
+  </si>
+  <si>
+    <t>failed</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +86,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -114,10 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D0B6B7-783B-4197-95AC-B82D60A80A6B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,6 +499,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>